<commit_message>
New dialog for importing examples - shows explanation and defaults the first prompt template.
</commit_message>
<xml_diff>
--- a/public/example/Examples.xlsx
+++ b/public/example/Examples.xlsx
@@ -5,6 +5,10 @@
   <sheets>
     <sheet state="visible" name="Pets I Own" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Christmas Decisions" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Submarine Support" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Office Feedback" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Failure to Launch" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="_meta" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="226">
   <si>
     <t>Name</t>
   </si>
@@ -26,7 +30,7 @@
     <t>Fido</t>
   </si>
   <si>
-    <t>Dog</t>
+    <t>dog</t>
   </si>
   <si>
     <t>benevolent</t>
@@ -35,7 +39,7 @@
     <t>Crumbers</t>
   </si>
   <si>
-    <t>Ferret</t>
+    <t>ferret</t>
   </si>
   <si>
     <t>sneaky</t>
@@ -50,7 +54,7 @@
     <t>Emilia</t>
   </si>
   <si>
-    <t>Parrot</t>
+    <t>parrot</t>
   </si>
   <si>
     <t>noisy</t>
@@ -65,7 +69,7 @@
     <t>Merlin</t>
   </si>
   <si>
-    <t>Cat</t>
+    <t>cat</t>
   </si>
   <si>
     <t>deceptive</t>
@@ -270,16 +274,452 @@
   </si>
   <si>
     <t>Science experiments, STEM kits, robotics</t>
+  </si>
+  <si>
+    <t>Ticket#</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Missing propeller in shipment</t>
+  </si>
+  <si>
+    <t>Customer reports missing propeller in shipment for personal submarine product, order number #SUB1234, received on 2023-02-20. The customer claims the propeller was not included in the package and the submarine is inoperable without it. The customer requests immediate assistance to resolve the issue and receive the missing propeller.</t>
+  </si>
+  <si>
+    <t>Confusing assembly manual for navigation system</t>
+  </si>
+  <si>
+    <t>The customer is experiencing difficulty navigating their personal submarine due to unclear instructions in the assembly manual, specifically the steps for configuring the sonar system and setting the depth gauge, which are not adequately explained or illustrated, leading to frustration and safety concerns.</t>
+  </si>
+  <si>
+    <t>Delayed delivery of submarine by two weeks</t>
+  </si>
+  <si>
+    <t>The customer reports that their personal submarine, ordered with an expected delivery date of 2 weeks ago, has yet to arrive. The customer has received no updates or communication from the manufacturer regarding the delay, and is now concerned about the impact on their planned underwater exploration trip. The customer requests immediate assistance in resolving the delivery issue and obtaining a revised delivery date.</t>
+  </si>
+  <si>
+    <t>Battery missing from packaging</t>
+  </si>
+  <si>
+    <t>The customer reports that upon opening the packaging for their personal submarine, they found that the battery was not included, which is a critical component for the device's operation. The customer is unable to use the submarine without the battery, and is requesting assistance with obtaining the missing part. The customer's order number is provided for reference.</t>
+  </si>
+  <si>
+    <t>Navigation software crashes during setup</t>
+  </si>
+  <si>
+    <t>Customer reports that during the setup process of our personal submarine's navigation software, the application crashes consistently when attempting to load the 3D map of the surrounding area. The error occurs when the software tries to render the map's underwater terrain, resulting in a system freeze and subsequent shutdown. Customer has tried restarting the system and reinstalling the software, but the issue persists.</t>
+  </si>
+  <si>
+    <t>Leaks detected in main hatch seal</t>
+  </si>
+  <si>
+    <t>Customer reports leaks detected in main hatch seal of their personal submarine, stating that during a recent dive, water began seeping into the vessel through the hatch area, causing the pressure gauge to fluctuate and the vessel to lose buoyancy.</t>
+  </si>
+  <si>
+    <t>Missing screws for propeller installation</t>
+  </si>
+  <si>
+    <t>The customer reports that the propeller installation kit for their personal submarine is incomplete, specifically missing the necessary screws required for secure attachment. The customer has confirmed that the propeller itself is present, but the screws are not, hindering the installation process. The customer requests assistance in resolving this issue to proceed with the propeller installation.</t>
+  </si>
+  <si>
+    <t>Poorly labeled parts in assembly kit</t>
+  </si>
+  <si>
+    <t>Customer reports that the assembly kit for the personal submarine contains parts that are not clearly labeled, making it difficult to identify and assemble the correct components. Specifically, the customer mentions that the 'Main Hull' and 'Control Panel' parts are incorrectly labeled as 'Left Hull' and 'Right Panel' respectively. This has resulted in the customer incorrectly assembling the submarine, which is now inoperable.</t>
+  </si>
+  <si>
+    <t>Depth gauge not functioning as expected</t>
+  </si>
+  <si>
+    <t>The customer reports that the depth gauge on their personal submarine is not functioning as expected, displaying inconsistent and inaccurate readings, and sometimes freezing altogether during dives. The issue occurs regardless of the water conditions, and the customer has tried resetting the gauge and checking the calibration but the problem persists. The customer is concerned that the inaccurate readings may compromise the safety of their dives.</t>
+  </si>
+  <si>
+    <t>Incorrect model delivered to customer</t>
+  </si>
+  <si>
+    <t>Customer received a personal submarine with a model number of 'PS-1000', but the actual model delivered was 'PS-500', which has a significantly reduced range and depth capabilities, causing inconvenience to the customer's planned underwater excursion.</t>
+  </si>
+  <si>
+    <t>Lights in cabin not turning on</t>
+  </si>
+  <si>
+    <t>Customer reports that the interior lights in their personal submarine's cabin are not functioning. The customer has checked the power switch and confirmed that it is in the 'on' position, but the lights remain dark. The issue is specific to the cabin lights, with all other systems functioning normally.</t>
+  </si>
+  <si>
+    <t>Propeller shaft misaligned during assembly</t>
+  </si>
+  <si>
+    <t>Customer reports that during the assembly of their personal submarine, the propeller shaft was incorrectly aligned, resulting in a 3-inch offset from the intended position. This misalignment is causing a 10% reduction in propulsion efficiency and a noticeable vibration during operation. Customer requests assistance with correcting the issue to ensure safe and optimal performance.</t>
+  </si>
+  <si>
+    <t>Shipping container damaged on arrival</t>
+  </si>
+  <si>
+    <t>Customer reports that the shipping container for their personal submarine was damaged upon arrival, resulting in scratches and dents on the vessel's exterior. The customer claims that the damage occurred during transit and that the container was not properly sealed, allowing water to enter and cause further damage. The customer requests a replacement container and expedited repair of the damaged vessel.</t>
+  </si>
+  <si>
+    <t>User manual missing from the box</t>
+  </si>
+  <si>
+    <t>Customer reports that the user manual for the personal submarine (model PS-1000) was not included in the packaging, making it difficult to understand and troubleshoot the device's operation, particularly the safety features and emergency procedures.</t>
+  </si>
+  <si>
+    <t>Submarine takes longer to charge than advertised</t>
+  </si>
+  <si>
+    <t>The customer reports that their personal submarine, model 'DeepDive', is taking approximately 4 hours to charge, whereas the product's documentation and marketing materials advertised a charging time of 2 hours. The customer has tried restarting the submarine and the charging station, but the issue persists. The customer is concerned that the prolonged charging time may impact their ability to use the submarine for extended periods.</t>
+  </si>
+  <si>
+    <t>Exterior paint chipped on arrival</t>
+  </si>
+  <si>
+    <t>Customer reports exterior paint chipped on arrival, specifically on the left side of the submersible, near the pressure hull. The chip is approximately 2 inches long and 1 inch wide, with visible metal underneath. Customer requests prompt repair or replacement to ensure water-tight integrity and prevent further damage.</t>
+  </si>
+  <si>
+    <t>Engine fails to start after assembly</t>
+  </si>
+  <si>
+    <t>Customer reports that after assembling the personal submarine, the engine fails to start. Upon further investigation, it appears that the fuel pump was not properly seated, preventing the engine from receiving the necessary fuel to initiate the start sequence. The customer has confirmed that the issue is resolved after re-seating the fuel pump and attempting to start the engine again.</t>
+  </si>
+  <si>
+    <t>GPS system does not acquire signal underwater</t>
+  </si>
+  <si>
+    <t>The customer reports that the GPS system on their personal submarine fails to acquire a signal when submerged, resulting in inaccurate location tracking and navigation. They mention that the issue occurs consistently in both shallow and deep water environments, and that the system's LED indicators do not display any error messages or warnings. The customer has tried restarting the system and recalibrating the GPS antenna, but the problem persists.</t>
+  </si>
+  <si>
+    <t>Cabin heating system not operational</t>
+  </si>
+  <si>
+    <t>Customer reports that the cabin heating system on their personal submarine is not operational, specifically stating that the temperature gauge remains at 0°F (0°C) despite the system being turned on and the heater being set to maximum. The customer has tried restarting the system and checking the circuit breaker, but the issue persists. The submarine's log shows no error messages related to the heating system, but the customer is concerned about the potential for hypothermia in cold water conditions.</t>
+  </si>
+  <si>
+    <t>Broken periscope lens in shipment</t>
+  </si>
+  <si>
+    <t>The customer reports that the periscope lens on their personal submarine is cracked and non-functional, which they claim was damaged during shipment. The customer states that the lens was in working order when they first inspected the submarine before the issue occurred. The customer requests a replacement lens or repair of the existing one to be expedited as soon as possible.</t>
+  </si>
+  <si>
+    <t>Control panel buttons not responding</t>
+  </si>
+  <si>
+    <t>Customer is experiencing issues with the control panel buttons on their personal submarine not responding. The buttons appear to be non-functional, preventing the customer from navigating the submarine or accessing critical systems. The customer has tried restarting the system, but the issue persists.</t>
+  </si>
+  <si>
+    <t>Misleading advertisement about speed capabilities</t>
+  </si>
+  <si>
+    <t>The customer is reporting that an advertisement for our personal submarine product claims it can reach speeds of up to 25 knots, but after purchasing the unit, they found that it can only maintain a speed of around 10 knots in calm waters, which they feel is misleading and not in line with the product's actual performance.</t>
+  </si>
+  <si>
+    <t>Weight limit lower than specified in manual</t>
+  </si>
+  <si>
+    <t>Dear Support Team, I'm experiencing an issue with my personal submarine, where the weight limit is lower than what's specified in the manual. When I loaded 3 passengers (total weight: 750 lbs) and 2 oxygen tanks (total weight: 200 lbs), the vessel's buoyancy system failed to compensate, causing the sub to sink rapidly. I'm concerned this discrepancy will compromise the safety of future dives.</t>
+  </si>
+  <si>
+    <t>Incomplete assembly kit provided</t>
+  </si>
+  <si>
+    <t>The customer received an incomplete assembly kit for their personal submarine, missing critical components such as the propulsion system, control panel, and emergency oxygen supply, rendering the product unusable.</t>
+  </si>
+  <si>
+    <t>Sonar system not providing accurate readings</t>
+  </si>
+  <si>
+    <t>The customer reports that the Sonar system on their personal submarine is consistently displaying inaccurate depth readings, often showing a discrepancy of 5-10 meters from the actual depth. This issue has been occurring during both shallow and deep dives, and the customer has tried restarting the system and recalibrating the sensors without resolving the problem. The customer is concerned that this inaccuracy may lead to navigation errors and potential safety risks.</t>
+  </si>
+  <si>
+    <t>Customer injured during assembly due to sharp edges</t>
+  </si>
+  <si>
+    <t>Customer was assembling the personal submarine when they cut their hand on a sharp edge on the control panel. The injury occurred while attempting to attach the control panel to the main hull, and the customer claims the edge was not adequately protected. The customer is requesting a replacement control panel with rounded edges to prevent future injuries.</t>
+  </si>
+  <si>
+    <t>Rubber seals missing for watertight doors</t>
+  </si>
+  <si>
+    <t>Customer reported that the watertight doors on their personal submarine are not functioning properly due to missing rubber seals, which is causing water to leak into the vessel during dives. The customer has tried to use the doors multiple times without success, resulting in minor flooding and concerns for safety. The issue is specific to the doors and not affecting other systems on the submarine.</t>
+  </si>
+  <si>
+    <t>Cabin size smaller than advertised</t>
+  </si>
+  <si>
+    <t>The customer reports that the cabin size of their personal submarine is approximately 2.5 feet in diameter and 4 feet in length, which is significantly smaller than the advertised 6 feet in diameter and 8 feet in length. This discrepancy is causing discomfort for the customer during extended dives. The customer requests a resolution to this issue, either through a refund or a complimentary upgrade to the correct model.</t>
+  </si>
+  <si>
+    <t>Fuel tank cap not sealing properly</t>
+  </si>
+  <si>
+    <t>The fuel tank cap on my personal submarine is not sealing properly, causing a slight hissing sound when I close it. I've tried cleaning the O-ring and ensuring it's properly seated, but the issue persists. The submarine is still operational, but I'm concerned that the leak may worsen over time if not addressed.</t>
+  </si>
+  <si>
+    <t>Customer received duplicate parts but missing others</t>
+  </si>
+  <si>
+    <t>Customer received a delivery containing duplicate parts (2 x thruster units) but was missing other essential components (1 x navigation system, 1 x communication device) required for the submarine's operation, which is causing a delay in their scheduled dive.</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Why does corporate not appreciate my leadership? I mean, I’m the World’s Best Boss—it's literally on my mug!</t>
+  </si>
+  <si>
+    <t>Jim</t>
+  </si>
+  <si>
+    <t>Can someone explain why I have to sit next to Dwight? He’s currently building a fort out of file folders to block my view.</t>
+  </si>
+  <si>
+    <t>Pam</t>
+  </si>
+  <si>
+    <t>Why does the copier break down every single time I need to print something important? It's like it knows.</t>
+  </si>
+  <si>
+    <t>Dwight</t>
+  </si>
+  <si>
+    <t>Michael doesn’t take my suggestions for improving office security seriously. I’ve sent him seven memos about nunchucks training.</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Why am I still the temp? I do everything around here—coffee runs, paper deliveries, and listening to Michael’s weird life advice.</t>
+  </si>
+  <si>
+    <t>Stanley</t>
+  </si>
+  <si>
+    <t>This office does not have decent chairs. My back is killing me, and I don’t even like standing up for pretzel day anymore.</t>
+  </si>
+  <si>
+    <t>Phyllis</t>
+  </si>
+  <si>
+    <t>Angela always criticizes my decorations. I think a little bit of sparkle in the office wouldn’t hurt anyone.</t>
+  </si>
+  <si>
+    <t>Angela</t>
+  </si>
+  <si>
+    <t>Why is the break room always so filthy? People need to respect that a communal space is not their personal dump.</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Seriously, there's never enough M&amp;M’s in the vending machine. I check every day, and every day I’m disappointed.</t>
+  </si>
+  <si>
+    <t>Oscar</t>
+  </si>
+  <si>
+    <t>Why does no one else here understand basic accounting principles? It's like I’m the only professional in a circus.</t>
+  </si>
+  <si>
+    <t>Meredith</t>
+  </si>
+  <si>
+    <t>Do we really need a policy against drinking at work? Sometimes you need a little nip to get through the day.</t>
+  </si>
+  <si>
+    <t>Creed</t>
+  </si>
+  <si>
+    <t>Too many rules about what you can and cannot take from the office. That’s what’s killing innovation.</t>
+  </si>
+  <si>
+    <t>Toby</t>
+  </si>
+  <si>
+    <t>I would just like Michael to treat me like a human being. Every time I speak, it’s like I’ve personally ruined his life.</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Why do we have to focus so much on paper? It’s 2005! Can’t we do something exciting, like designing celebrity stationery?</t>
+  </si>
+  <si>
+    <t>Launch Failure Date</t>
+  </si>
+  <si>
+    <t>Engineer's Report</t>
+  </si>
+  <si>
+    <t>Site Manager's Report</t>
+  </si>
+  <si>
+    <t>Janitor's Report</t>
+  </si>
+  <si>
+    <t>Preliminary diagnostics indicate a critical failure in the primary engine's turbopump assembly, likely due to cavitation-induced wear leading to suboptimal fuel flow rates.</t>
+  </si>
+  <si>
+    <t>unavailable</t>
+  </si>
+  <si>
+    <t>I saw some guys looking at a pipe and shaking their heads a lot.</t>
+  </si>
+  <si>
+    <t>Faulty sensor in the guidance system has been flagged; engineers are investigating.</t>
+  </si>
+  <si>
+    <t>There was a blinking light on a computer, and someone seemed pretty mad about it.</t>
+  </si>
+  <si>
+    <t>Structural analysis reveals microfractures in the rocket's outer shell at stress concentration points, exacerbated by thermal cycling during testing.</t>
+  </si>
+  <si>
+    <t>No assessment given.</t>
+  </si>
+  <si>
+    <t>The rocket looked kind of bent in one spot, but I’m not sure if that’s normal.</t>
+  </si>
+  <si>
+    <t>I was absent from the point of failure.</t>
+  </si>
+  <si>
+    <t>Hydraulic system failure in the landing gear has been reported; cause is unclear.</t>
+  </si>
+  <si>
+    <t>A bunch of fluid sprayed out of something under the rocket, and people started running around.</t>
+  </si>
+  <si>
+    <t>Communication issues from link station 33.</t>
+  </si>
+  <si>
+    <t>Some of the walkie-talkies weren’t working; I think someone said something about static.</t>
+  </si>
+  <si>
+    <t>Meteorological data confirms sustained wind velocities exceeding 45 knots at 200-meter altitudes, breaching the launch safety threshold for stability.</t>
+  </si>
+  <si>
+    <t>High winds at the launch site exceed safety limits; we’ll delay until conditions improve.</t>
+  </si>
+  <si>
+    <t>The wind was blowing really hard, and someone’s hat flew off.</t>
+  </si>
+  <si>
+    <t>Electrostatic discharge modeling predicts a 70% probability of lightning strikes in the vicinity, triggered by elevated atmospheric instability near the launch pad.</t>
+  </si>
+  <si>
+    <t>I saw lightning way off in the distance, and then everyone started talking about delays.</t>
+  </si>
+  <si>
+    <t>The absence of the propulsion specialist due to an unanticipated medical emergency has delayed critical system validations for main engine synchronization.</t>
+  </si>
+  <si>
+    <t>A key propulsion technician is absent due to a medical emergency; testing is paused.</t>
+  </si>
+  <si>
+    <t>One of the workers wasn’t there, and someone said he was sick or something.</t>
+  </si>
+  <si>
+    <t>No technical faults observed. Protocol-related.</t>
+  </si>
+  <si>
+    <t>Safety protocol was not followed by a crew member; retraining is being scheduled.</t>
+  </si>
+  <si>
+    <t>Some guy opened the wrong door, and people started yelling about safety.</t>
+  </si>
+  <si>
+    <t>Anomalous readings in telemetry data suggest a possible fault in the primary avionics suite, but the exact subsystem involved remains indeterminate at this stage.</t>
+  </si>
+  <si>
+    <t>Further investigation needed. Root cause unclear.</t>
+  </si>
+  <si>
+    <t>They said some numbers on the computer didn’t match up, and no one knew why.</t>
+  </si>
+  <si>
+    <t>Sheet Name</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>Default Prompt</t>
+  </si>
+  <si>
+    <t>Pets I Own</t>
+  </si>
+  <si>
+    <t>When you have a lot of pets, you need a spreadsheet to keep track of them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I want to give {Name}, my pet {Animal}, a new Spanish name that reflects their {Disposition} personality. Output a single name. </t>
+  </si>
+  <si>
+    <t>Christmas Decisions</t>
+  </si>
+  <si>
+    <t>Can we be more efficient and objective in planning gifts for children?</t>
+  </si>
+  <si>
+    <t>If Santa received feedback of "{Feedback}" for a child, how should he judge the child? Output the single word of "naughty" or "nice".</t>
+  </si>
+  <si>
+    <t>Submarine Support</t>
+  </si>
+  <si>
+    <t>Customers are having trouble with our submarine product. What can we learn from them?</t>
+  </si>
+  <si>
+    <t>Summary: {Summary}
+Details: {Details}
+Choose the best classification of the customer's problem and output just one of the following codes: "ordering", "payment", "delivery", "assembly", "operation", or "other"</t>
+  </si>
+  <si>
+    <t>Office Feedback</t>
+  </si>
+  <si>
+    <t>Our "anonymous" feedback jar filled up quickly. But it's painfully easy to see who said what.</t>
+  </si>
+  <si>
+    <t>Feedback: {Feedback}
+Summarize the employee feedback in one sentence of less than 10 words. Roles, names of people, and specific events should be removed or made vague to keep the identity of the employee anonymous.</t>
+  </si>
+  <si>
+    <t>Failure to Launch</t>
+  </si>
+  <si>
+    <t>When our rockets fail to launch, we gather data. Does it tell us the cause?</t>
+  </si>
+  <si>
+    <t>Consider the reports below concerning a failed rocket launch. In less than 6 words, summarize the cause of failure.
+Engineer: "{Engineer's Report}"
+Site Manager: "{Site Manager's Report}"
+Janitor: "{Janitor's Report}"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="M/d/yyyy"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -291,6 +731,12 @@
     <font>
       <b/>
       <u/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -310,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -319,6 +765,18 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -333,6 +791,22 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -552,90 +1026,90 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -659,234 +1133,994 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="8.75"/>
+    <col customWidth="1" min="2" max="2" width="42.0"/>
+    <col customWidth="1" min="3" max="3" width="24.88"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2">
+        <v>1460.0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2">
+        <v>1461.0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2">
+        <v>1462.0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2">
+        <v>1463.0</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2">
+        <v>1464.0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2">
+        <v>1465.0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2">
+        <v>1466.0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2">
+        <v>1467.0</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2">
+        <v>1468.0</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2">
+        <v>1469.0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2">
+        <v>1470.0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2">
+        <v>1471.0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2">
+        <v>1472.0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2">
+        <v>1473.0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2">
+        <v>1474.0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2">
+        <v>1475.0</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2">
+        <v>1476.0</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2">
+        <v>1477.0</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2">
+        <v>1478.0</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2">
+        <v>1479.0</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2">
+        <v>1480.0</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2">
+        <v>1481.0</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2">
+        <v>1482.0</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2">
+        <v>1483.0</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2">
+        <v>1484.0</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2">
+        <v>1485.0</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2">
+        <v>1486.0</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2">
+        <v>1487.0</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2">
+        <v>1488.0</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2">
+        <v>1489.0</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="95.75"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="18.0"/>
+    <col customWidth="1" min="2" max="2" width="50.13"/>
+    <col customWidth="1" min="3" max="3" width="46.25"/>
+    <col customWidth="1" min="4" max="4" width="40.38"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5">
+        <v>49605.0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5">
+        <v>48199.0</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5">
+        <v>47971.0</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5">
+        <v>49561.0</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5">
+        <v>48831.0</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5">
+        <v>50014.0</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5">
+        <v>51083.0</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="5">
+        <v>48224.0</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="5">
+        <v>49418.0</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="5">
+        <v>49664.0</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="18.75"/>
+    <col customWidth="1" min="2" max="3" width="63.75"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>225</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Don't need the start screen. Things work better without it.
</commit_message>
<xml_diff>
--- a/public/example/Examples.xlsx
+++ b/public/example/Examples.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="236">
   <si>
     <t>Name</t>
   </si>
@@ -561,6 +561,9 @@
     <t>Janitor's Report</t>
   </si>
   <si>
+    <t>10/23/2035</t>
+  </si>
+  <si>
     <t>Preliminary diagnostics indicate a critical failure in the primary engine's turbopump assembly, likely due to cavitation-induced wear leading to suboptimal fuel flow rates.</t>
   </si>
   <si>
@@ -570,12 +573,18 @@
     <t>I saw some guys looking at a pipe and shaking their heads a lot.</t>
   </si>
   <si>
+    <t>12/17/2031</t>
+  </si>
+  <si>
     <t>Faulty sensor in the guidance system has been flagged; engineers are investigating.</t>
   </si>
   <si>
     <t>There was a blinking light on a computer, and someone seemed pretty mad about it.</t>
   </si>
   <si>
+    <t>5/3/2031</t>
+  </si>
+  <si>
     <t>Structural analysis reveals microfractures in the rocket's outer shell at stress concentration points, exacerbated by thermal cycling during testing.</t>
   </si>
   <si>
@@ -585,6 +594,9 @@
     <t>The rocket looked kind of bent in one spot, but I’m not sure if that’s normal.</t>
   </si>
   <si>
+    <t>9/9/2035</t>
+  </si>
+  <si>
     <t>I was absent from the point of failure.</t>
   </si>
   <si>
@@ -594,12 +606,18 @@
     <t>A bunch of fluid sprayed out of something under the rocket, and people started running around.</t>
   </si>
   <si>
+    <t>9/9/2033</t>
+  </si>
+  <si>
     <t>Communication issues from link station 33.</t>
   </si>
   <si>
     <t>Some of the walkie-talkies weren’t working; I think someone said something about static.</t>
   </si>
   <si>
+    <t>12/5/2036</t>
+  </si>
+  <si>
     <t>Meteorological data confirms sustained wind velocities exceeding 45 knots at 200-meter altitudes, breaching the launch safety threshold for stability.</t>
   </si>
   <si>
@@ -609,12 +627,18 @@
     <t>The wind was blowing really hard, and someone’s hat flew off.</t>
   </si>
   <si>
+    <t>11/9/2039</t>
+  </si>
+  <si>
     <t>Electrostatic discharge modeling predicts a 70% probability of lightning strikes in the vicinity, triggered by elevated atmospheric instability near the launch pad.</t>
   </si>
   <si>
     <t>I saw lightning way off in the distance, and then everyone started talking about delays.</t>
   </si>
   <si>
+    <t>1/11/2032</t>
+  </si>
+  <si>
     <t>The absence of the propulsion specialist due to an unanticipated medical emergency has delayed critical system validations for main engine synchronization.</t>
   </si>
   <si>
@@ -624,6 +648,9 @@
     <t>One of the workers wasn’t there, and someone said he was sick or something.</t>
   </si>
   <si>
+    <t>4/19/2035</t>
+  </si>
+  <si>
     <t>No technical faults observed. Protocol-related.</t>
   </si>
   <si>
@@ -631,6 +658,9 @@
   </si>
   <si>
     <t>Some guy opened the wrong door, and people started yelling about safety.</t>
+  </si>
+  <si>
+    <t>12/21/2035</t>
   </si>
   <si>
     <t>Anomalous readings in telemetry data suggest a possible fault in the primary avionics suite, but the exact subsystem involved remains indeterminate at this stage.</t>
@@ -706,9 +736,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="M/d/yyyy"/>
-  </numFmts>
   <fonts count="5">
     <font>
       <sz val="10.0"/>
@@ -772,7 +799,7 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1899,143 +1926,143 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5">
-        <v>49605.0</v>
+      <c r="A2" s="5" t="s">
+        <v>181</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5">
-        <v>48199.0</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>182</v>
-      </c>
       <c r="C3" s="6" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="5">
-        <v>47971.0</v>
+      <c r="A4" s="5" t="s">
+        <v>188</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="5">
-        <v>49561.0</v>
+      <c r="A5" s="5" t="s">
+        <v>192</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="5">
-        <v>48831.0</v>
+      <c r="A6" s="5" t="s">
+        <v>196</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5">
-        <v>50014.0</v>
+      <c r="A7" s="5" t="s">
+        <v>199</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="5">
-        <v>51083.0</v>
+      <c r="A8" s="5" t="s">
+        <v>203</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="5">
-        <v>48224.0</v>
+      <c r="A9" s="5" t="s">
+        <v>206</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>200</v>
+        <v>208</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="5">
-        <v>49418.0</v>
+      <c r="A10" s="5" t="s">
+        <v>210</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="5">
-        <v>49664.0</v>
+      <c r="A11" s="5" t="s">
+        <v>214</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2059,68 +2086,68 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>

</xml_diff>